<commit_message>
Changed style of table in xlsx file
</commit_message>
<xml_diff>
--- a/plot.xlsx
+++ b/plot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itmo_lab\lab3\lab3_new\lab3_with_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DCAA522-8E3E-41B2-8E40-5CD555CC9E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39E619C-C9B9-4512-B920-E1A0B3B25F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F40DAE26-AB96-462B-B72F-869E7956BDD9}"/>
   </bookViews>
@@ -71,17 +71,100 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -91,9 +174,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1505,7 +1599,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1515,147 +1609,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="12">
         <v>4</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="2">
         <v>8</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="2">
         <v>16</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="2">
         <v>20</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="2">
         <v>25</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="2">
         <v>30</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="2">
         <v>32</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="2">
         <v>35</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="2">
         <v>64</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="2">
         <v>128</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="2">
         <v>250</v>
       </c>
-      <c r="M1">
+      <c r="M1" s="2">
         <v>500</v>
       </c>
-      <c r="N1">
+      <c r="N1" s="2">
         <v>1000</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="3">
         <v>2000</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <f>0.0000001*10^(9)</f>
         <v>100</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6">
         <v>200</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="6">
         <v>300</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="6">
         <v>300</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="6">
         <v>600</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="6">
         <v>500</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="6">
         <v>600</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="6">
         <v>700</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="6">
         <v>1400</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="6">
         <v>3700</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="6">
         <v>9600</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="6">
         <v>35500</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="6">
         <f>0.0001306*10^9</f>
         <v>130600</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="7">
         <f>0.0004946*10^9</f>
         <v>494600</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="8">
         <f>0.0000002*10^(9)</f>
         <v>200</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="9">
         <v>200</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="9">
         <v>400</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="9">
         <v>400</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="9">
         <v>400</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="9">
         <v>400</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="9">
         <v>500</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="9">
         <v>600</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="9">
         <v>700</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="9">
         <v>900</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="9">
         <v>1100</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="9">
         <v>1800</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="9">
         <v>3500</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="10">
         <v>7200</v>
       </c>
     </row>

</xml_diff>